<commit_message>
add file backup data
</commit_message>
<xml_diff>
--- a/Data/Data Value.xlsx
+++ b/Data/Data Value.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LOAI_SAN_PHAM" sheetId="1" r:id="rId1"/>
@@ -682,8 +682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -897,7 +897,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1016,7 +1016,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1148,7 +1148,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1301,7 +1301,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>